<commit_message>
feature: Added angle offset
</commit_message>
<xml_diff>
--- a/lidar_comparison/cone_hits.xlsx
+++ b/lidar_comparison/cone_hits.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,29 +444,13 @@
           <t>64 Channels, 45° FOV</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>128 Channels, 45° FOV</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>128 Channels, 22.5° FOV</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>6</v>
-      </c>
-      <c r="C2" t="n">
-        <v>12</v>
-      </c>
-      <c r="D2" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -476,12 +460,6 @@
       <c r="B3" t="n">
         <v>3</v>
       </c>
-      <c r="C3" t="n">
-        <v>6</v>
-      </c>
-      <c r="D3" t="n">
-        <v>13</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -490,12 +468,6 @@
       <c r="B4" t="n">
         <v>2</v>
       </c>
-      <c r="C4" t="n">
-        <v>4</v>
-      </c>
-      <c r="D4" t="n">
-        <v>9</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -504,12 +476,6 @@
       <c r="B5" t="n">
         <v>1</v>
       </c>
-      <c r="C5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D5" t="n">
-        <v>5</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -518,12 +484,6 @@
       <c r="B6" t="n">
         <v>1</v>
       </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" t="n">
-        <v>3</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -532,12 +492,6 @@
       <c r="B7" t="n">
         <v>1</v>
       </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -546,24 +500,12 @@
       <c r="B8" t="n">
         <v>0</v>
       </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" t="n">
-        <v>2</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
         <v>40</v>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: changed figure scaling
</commit_message>
<xml_diff>
--- a/lidar_comparison/cone_hits.xlsx
+++ b/lidar_comparison/cone_hits.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,6 +444,16 @@
           <t>64 Channels, 45° FOV</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>128 Channels, 45° FOV</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>128 Channels, 22.5° FOV</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -452,6 +462,12 @@
       <c r="B2" t="n">
         <v>0</v>
       </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -460,6 +476,12 @@
       <c r="B3" t="n">
         <v>3</v>
       </c>
+      <c r="C3" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3" t="n">
+        <v>13</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -468,6 +490,12 @@
       <c r="B4" t="n">
         <v>2</v>
       </c>
+      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -476,6 +504,12 @@
       <c r="B5" t="n">
         <v>1</v>
       </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -484,6 +518,12 @@
       <c r="B6" t="n">
         <v>1</v>
       </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -492,6 +532,12 @@
       <c r="B7" t="n">
         <v>1</v>
       </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -500,12 +546,24 @@
       <c r="B8" t="n">
         <v>0</v>
       </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
         <v>40</v>
       </c>
       <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feature: Add cone hits
</commit_message>
<xml_diff>
--- a/lidar_comparison/cone_hits.xlsx
+++ b/lidar_comparison/cone_hits.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,17 +441,37 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>64 Channels, 45° FOV</t>
+          <t>32 Channels OS1 Normal, 45° FOV</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>128 Channels, 45° FOV</t>
+          <t>64 Channels OS1 Normal, 45° FOV</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>128 Channels, 22.5° FOV</t>
+          <t>128 Channels OS1 Normal, 45° FOV</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>32 Channels OS1 Below Horizon, 22.5° FOV</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>64 Channels OS1 Below Horizon, 22.5° FOV</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>128 Channels OS1 Below Horizon, 22.5° FOV</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>128 Channels OS2 Normal, 22.5° FOV</t>
         </is>
       </c>
     </row>
@@ -468,18 +488,42 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>10</v>
       </c>
       <c r="B3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
         <v>3</v>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>6</v>
       </c>
-      <c r="D3" t="n">
+      <c r="E3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" t="n">
+        <v>7</v>
+      </c>
+      <c r="G3" t="n">
+        <v>13</v>
+      </c>
+      <c r="H3" t="n">
         <v>13</v>
       </c>
     </row>
@@ -488,12 +532,24 @@
         <v>15</v>
       </c>
       <c r="B4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
         <v>2</v>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>4</v>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" t="n">
+        <v>4</v>
+      </c>
+      <c r="G4" t="n">
+        <v>8</v>
+      </c>
+      <c r="H4" t="n">
         <v>9</v>
       </c>
     </row>
@@ -502,12 +558,24 @@
         <v>20</v>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
         <v>3</v>
       </c>
-      <c r="D5" t="n">
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H5" t="n">
         <v>5</v>
       </c>
     </row>
@@ -522,6 +590,18 @@
         <v>1</v>
       </c>
       <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>3</v>
+      </c>
+      <c r="H6" t="n">
         <v>3</v>
       </c>
     </row>
@@ -530,12 +610,24 @@
         <v>30</v>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" t="n">
         <v>1</v>
       </c>
       <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" t="n">
+        <v>2</v>
+      </c>
+      <c r="H7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -547,9 +639,21 @@
         <v>0</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="n">
         <v>2</v>
       </c>
     </row>
@@ -564,6 +668,18 @@
         <v>0</v>
       </c>
       <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>